<commit_message>
propensity score por 4º vez
</commit_message>
<xml_diff>
--- a/Outputs/Tablas_basales/Tabla_basal_sin_missings.xlsx
+++ b/Outputs/Tablas_basales/Tabla_basal_sin_missings.xlsx
@@ -351,7 +351,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:H99"/>
+  <dimension ref="A1:H106"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
@@ -429,7 +429,7 @@
       </c>
       <c r="C3" t="inlineStr">
         <is>
-          <t xml:space="preserve"> 26.95 [23.99, 30.41]</t>
+          <t xml:space="preserve"> 26.88 [23.97, 30.41]</t>
         </is>
       </c>
       <c r="D3" t="inlineStr">
@@ -439,12 +439,12 @@
       </c>
       <c r="E3" t="inlineStr">
         <is>
-          <t xml:space="preserve"> 26.64 [23.77, 30.48]</t>
+          <t xml:space="preserve"> 26.45 [23.73, 30.48]</t>
         </is>
       </c>
       <c r="F3" t="inlineStr">
         <is>
-          <t xml:space="preserve"> 0.214</t>
+          <t xml:space="preserve"> 0.182</t>
         </is>
       </c>
       <c r="G3" t="inlineStr">
@@ -454,7 +454,7 @@
       </c>
       <c r="H3" t="inlineStr">
         <is>
-          <t xml:space="preserve"> 0.139</t>
+          <t xml:space="preserve"> 0.146</t>
         </is>
       </c>
     </row>
@@ -503,7 +503,7 @@
       </c>
       <c r="F5" t="inlineStr">
         <is>
-          <t xml:space="preserve"> 0.048</t>
+          <t xml:space="preserve"> 0.050</t>
         </is>
       </c>
       <c r="G5" t="inlineStr">
@@ -513,7 +513,7 @@
       </c>
       <c r="H5" t="inlineStr">
         <is>
-          <t xml:space="preserve"> 0.172</t>
+          <t xml:space="preserve"> 0.171</t>
         </is>
       </c>
     </row>
@@ -557,12 +557,12 @@
       </c>
       <c r="E7" t="inlineStr">
         <is>
-          <t xml:space="preserve">  1.65 [1.58, 1.71]</t>
+          <t xml:space="preserve">  1.66 [1.59, 1.71]</t>
         </is>
       </c>
       <c r="F7" t="inlineStr">
         <is>
-          <t xml:space="preserve"> 0.297</t>
+          <t xml:space="preserve"> 0.410</t>
         </is>
       </c>
       <c r="G7" t="inlineStr">
@@ -572,7 +572,7 @@
       </c>
       <c r="H7" t="inlineStr">
         <is>
-          <t xml:space="preserve"> 0.100</t>
+          <t xml:space="preserve"> 0.078</t>
         </is>
       </c>
     </row>
@@ -729,7 +729,7 @@
       </c>
       <c r="D13" t="inlineStr">
         <is>
-          <t xml:space="preserve"> 44.50 [28.00, 78.75]</t>
+          <t xml:space="preserve"> 44.00 [28.00, 77.75]</t>
         </is>
       </c>
       <c r="E13" t="inlineStr">
@@ -749,7 +749,7 @@
       </c>
       <c r="H13" t="inlineStr">
         <is>
-          <t xml:space="preserve"> 0.500</t>
+          <t xml:space="preserve"> 0.485</t>
         </is>
       </c>
     </row>
@@ -793,7 +793,7 @@
       </c>
       <c r="E15" t="inlineStr">
         <is>
-          <t xml:space="preserve"> 31.00 [22.00, 51.00]</t>
+          <t xml:space="preserve"> 31.00 [21.00, 51.00]</t>
         </is>
       </c>
       <c r="F15" t="inlineStr">
@@ -842,22 +842,22 @@
       </c>
       <c r="C17" t="inlineStr">
         <is>
-          <t xml:space="preserve"> 37.60 [34.00, 41.00]</t>
+          <t xml:space="preserve"> 37.50 [34.00, 41.00]</t>
         </is>
       </c>
       <c r="D17" t="inlineStr">
         <is>
-          <t xml:space="preserve"> 37.00 [34.00, 40.53]</t>
+          <t xml:space="preserve"> 37.00 [34.00, 40.85]</t>
         </is>
       </c>
       <c r="E17" t="inlineStr">
         <is>
-          <t xml:space="preserve"> 38.30 [33.80, 41.20]</t>
+          <t xml:space="preserve"> 38.00 [33.80, 41.20]</t>
         </is>
       </c>
       <c r="F17" t="inlineStr">
         <is>
-          <t xml:space="preserve"> 0.463</t>
+          <t xml:space="preserve"> 0.610</t>
         </is>
       </c>
       <c r="G17" t="inlineStr">
@@ -867,7 +867,7 @@
       </c>
       <c r="H17" t="inlineStr">
         <is>
-          <t xml:space="preserve"> 0.030</t>
+          <t xml:space="preserve"> 0.048</t>
         </is>
       </c>
     </row>
@@ -901,17 +901,17 @@
       </c>
       <c r="C19" t="inlineStr">
         <is>
-          <t xml:space="preserve">  1.00 [0.70, 1.46]</t>
+          <t xml:space="preserve">  1.00 [0.70, 1.50]</t>
         </is>
       </c>
       <c r="D19" t="inlineStr">
         <is>
-          <t xml:space="preserve">  1.17 [0.82, 1.58]</t>
+          <t xml:space="preserve">  1.17 [0.83, 1.62]</t>
         </is>
       </c>
       <c r="E19" t="inlineStr">
         <is>
-          <t xml:space="preserve">  0.85 [0.63, 1.22]</t>
+          <t xml:space="preserve">  0.85 [0.63, 1.23]</t>
         </is>
       </c>
       <c r="F19" t="inlineStr">
@@ -926,7 +926,7 @@
       </c>
       <c r="H19" t="inlineStr">
         <is>
-          <t xml:space="preserve"> 0.259</t>
+          <t xml:space="preserve"> 0.257</t>
         </is>
       </c>
     </row>
@@ -1034,7 +1034,7 @@
       </c>
       <c r="F23" t="inlineStr">
         <is>
-          <t xml:space="preserve"> 0.070</t>
+          <t xml:space="preserve"> 0.068</t>
         </is>
       </c>
       <c r="G23" t="inlineStr">
@@ -1044,7 +1044,7 @@
       </c>
       <c r="H23" t="inlineStr">
         <is>
-          <t xml:space="preserve"> 0.335</t>
+          <t xml:space="preserve"> 0.336</t>
         </is>
       </c>
     </row>
@@ -1078,22 +1078,22 @@
       </c>
       <c r="C25" t="inlineStr">
         <is>
-          <t xml:space="preserve"> 99.00 [75.50, 141.00]</t>
+          <t xml:space="preserve"> 99.00 [74.00, 135.00]</t>
         </is>
       </c>
       <c r="D25" t="inlineStr">
         <is>
-          <t>101.50 [79.00, 148.75]</t>
+          <t>101.00 [77.25, 140.50]</t>
         </is>
       </c>
       <c r="E25" t="inlineStr">
         <is>
-          <t xml:space="preserve"> 92.00 [72.00, 132.00]</t>
+          <t xml:space="preserve"> 91.00 [72.00, 122.00]</t>
         </is>
       </c>
       <c r="F25" t="inlineStr">
         <is>
-          <t xml:space="preserve"> 0.028</t>
+          <t xml:space="preserve"> 0.019</t>
         </is>
       </c>
       <c r="G25" t="inlineStr">
@@ -1103,7 +1103,7 @@
       </c>
       <c r="H25" t="inlineStr">
         <is>
-          <t xml:space="preserve"> 0.069</t>
+          <t xml:space="preserve"> 0.045</t>
         </is>
       </c>
     </row>
@@ -1132,22 +1132,22 @@
     <row r="27">
       <c r="A27" t="inlineStr">
         <is>
-          <t>FsC_Elastografia (median [IQR])</t>
+          <t>FsC (median [IQR])</t>
         </is>
       </c>
       <c r="C27" t="inlineStr">
         <is>
-          <t xml:space="preserve"> 22.00 [14.30, 35.30]</t>
+          <t xml:space="preserve"> 22.15 [14.10, 35.17]</t>
         </is>
       </c>
       <c r="D27" t="inlineStr">
         <is>
-          <t xml:space="preserve"> 27.35 [17.30, 43.12]</t>
+          <t xml:space="preserve"> 28.50 [18.90, 39.60]</t>
         </is>
       </c>
       <c r="E27" t="inlineStr">
         <is>
-          <t xml:space="preserve"> 20.00 [13.60, 32.00]</t>
+          <t xml:space="preserve"> 17.15 [11.83, 22.23]</t>
         </is>
       </c>
       <c r="F27" t="inlineStr">
@@ -1162,56 +1162,56 @@
       </c>
       <c r="H27" t="inlineStr">
         <is>
-          <t xml:space="preserve"> 0.428</t>
+          <t xml:space="preserve"> 0.698</t>
         </is>
       </c>
     </row>
     <row r="28">
       <c r="A28" t="inlineStr">
         <is>
-          <t>FsC_Elastografia (missing values)</t>
+          <t>FsC (missing values)</t>
         </is>
       </c>
       <c r="C28" t="inlineStr">
         <is>
-          <t>0</t>
+          <t>189</t>
         </is>
       </c>
       <c r="D28" t="inlineStr">
         <is>
-          <t>0</t>
+          <t>90</t>
         </is>
       </c>
       <c r="E28" t="inlineStr">
         <is>
-          <t>0</t>
+          <t>99</t>
         </is>
       </c>
     </row>
     <row r="29">
       <c r="A29" t="inlineStr">
         <is>
-          <t>GGT_preIQ (median [IQR])</t>
+          <t>FsC_Elastografia (median [IQR])</t>
         </is>
       </c>
       <c r="C29" t="inlineStr">
         <is>
-          <t xml:space="preserve"> 75.00 [41.00, 129.50]</t>
+          <t xml:space="preserve"> 22.30 [14.10, 35.30]</t>
         </is>
       </c>
       <c r="D29" t="inlineStr">
         <is>
-          <t xml:space="preserve"> 74.50 [46.25, 120.00]</t>
+          <t xml:space="preserve"> 26.80 [17.30, 36.17]</t>
         </is>
       </c>
       <c r="E29" t="inlineStr">
         <is>
-          <t xml:space="preserve"> 77.00 [36.00, 137.00]</t>
+          <t xml:space="preserve"> 20.60 [14.00, 34.00]</t>
         </is>
       </c>
       <c r="F29" t="inlineStr">
         <is>
-          <t xml:space="preserve"> 0.887</t>
+          <t>&lt;0.001</t>
         </is>
       </c>
       <c r="G29" t="inlineStr">
@@ -1221,14 +1221,14 @@
       </c>
       <c r="H29" t="inlineStr">
         <is>
-          <t xml:space="preserve"> 0.192</t>
+          <t xml:space="preserve"> 0.290</t>
         </is>
       </c>
     </row>
     <row r="30">
       <c r="A30" t="inlineStr">
         <is>
-          <t>GGT_preIQ (missing values)</t>
+          <t>FsC_Elastografia (missing values)</t>
         </is>
       </c>
       <c r="C30" t="inlineStr">
@@ -1250,27 +1250,27 @@
     <row r="31">
       <c r="A31" t="inlineStr">
         <is>
-          <t>INR_preIQ (median [IQR])</t>
+          <t>GGT_preIQ (median [IQR])</t>
         </is>
       </c>
       <c r="C31" t="inlineStr">
         <is>
-          <t xml:space="preserve">  1.14 [1.06, 1.24]</t>
+          <t xml:space="preserve"> 74.00 [41.00, 128.00]</t>
         </is>
       </c>
       <c r="D31" t="inlineStr">
         <is>
-          <t xml:space="preserve">  1.16 [1.09, 1.27]</t>
+          <t xml:space="preserve"> 73.00 [42.25, 111.75]</t>
         </is>
       </c>
       <c r="E31" t="inlineStr">
         <is>
-          <t xml:space="preserve">  1.12 [1.03, 1.21]</t>
+          <t xml:space="preserve"> 77.00 [38.00, 140.00]</t>
         </is>
       </c>
       <c r="F31" t="inlineStr">
         <is>
-          <t>&lt;0.001</t>
+          <t xml:space="preserve"> 0.335</t>
         </is>
       </c>
       <c r="G31" t="inlineStr">
@@ -1280,14 +1280,14 @@
       </c>
       <c r="H31" t="inlineStr">
         <is>
-          <t xml:space="preserve"> 0.184</t>
+          <t xml:space="preserve"> 0.205</t>
         </is>
       </c>
     </row>
     <row r="32">
       <c r="A32" t="inlineStr">
         <is>
-          <t>INR_preIQ (missing values)</t>
+          <t>GGT_preIQ (missing values)</t>
         </is>
       </c>
       <c r="C32" t="inlineStr">
@@ -1309,27 +1309,27 @@
     <row r="33">
       <c r="A33" t="inlineStr">
         <is>
-          <t>MELD_basal (median [IQR])</t>
+          <t>INR_preIQ (median [IQR])</t>
         </is>
       </c>
       <c r="C33" t="inlineStr">
         <is>
-          <t xml:space="preserve">  8.93 [7.60, 10.34]</t>
+          <t xml:space="preserve">  1.14 [1.06, 1.23]</t>
         </is>
       </c>
       <c r="D33" t="inlineStr">
         <is>
-          <t xml:space="preserve">  9.04 [7.93, 10.46]</t>
+          <t xml:space="preserve">  1.16 [1.09, 1.26]</t>
         </is>
       </c>
       <c r="E33" t="inlineStr">
         <is>
-          <t xml:space="preserve">  8.00 [7.00, 10.00]</t>
+          <t xml:space="preserve">  1.12 [1.03, 1.21]</t>
         </is>
       </c>
       <c r="F33" t="inlineStr">
         <is>
-          <t xml:space="preserve"> 0.005</t>
+          <t>&lt;0.001</t>
         </is>
       </c>
       <c r="G33" t="inlineStr">
@@ -1339,14 +1339,14 @@
       </c>
       <c r="H33" t="inlineStr">
         <is>
-          <t xml:space="preserve"> 0.045</t>
+          <t xml:space="preserve"> 0.178</t>
         </is>
       </c>
     </row>
     <row r="34">
       <c r="A34" t="inlineStr">
         <is>
-          <t>MELD_basal (missing values)</t>
+          <t>INR_preIQ (missing values)</t>
         </is>
       </c>
       <c r="C34" t="inlineStr">
@@ -1368,27 +1368,27 @@
     <row r="35">
       <c r="A35" t="inlineStr">
         <is>
-          <t>MidaMelsa_mm (median [IQR])</t>
+          <t>MELD_basal (median [IQR])</t>
         </is>
       </c>
       <c r="C35" t="inlineStr">
         <is>
-          <t>138.00 [120.00, 155.50]</t>
+          <t xml:space="preserve">  8.88 [7.56, 10.34]</t>
         </is>
       </c>
       <c r="D35" t="inlineStr">
         <is>
-          <t>140.00 [130.00, 160.00]</t>
+          <t xml:space="preserve">  9.02 [7.91, 10.46]</t>
         </is>
       </c>
       <c r="E35" t="inlineStr">
         <is>
-          <t>129.00 [120.00, 150.00]</t>
+          <t xml:space="preserve">  8.00 [7.00, 10.00]</t>
         </is>
       </c>
       <c r="F35" t="inlineStr">
         <is>
-          <t xml:space="preserve"> 0.001</t>
+          <t xml:space="preserve"> 0.006</t>
         </is>
       </c>
       <c r="G35" t="inlineStr">
@@ -1398,14 +1398,14 @@
       </c>
       <c r="H35" t="inlineStr">
         <is>
-          <t xml:space="preserve"> 0.214</t>
+          <t xml:space="preserve"> 0.041</t>
         </is>
       </c>
     </row>
     <row r="36">
       <c r="A36" t="inlineStr">
         <is>
-          <t>MidaMelsa_mm (missing values)</t>
+          <t>MELD_basal (missing values)</t>
         </is>
       </c>
       <c r="C36" t="inlineStr">
@@ -1427,27 +1427,27 @@
     <row r="37">
       <c r="A37" t="inlineStr">
         <is>
-          <t>Pughpunts_basal (median [IQR])</t>
+          <t>MidaMelsa_mm (median [IQR])</t>
         </is>
       </c>
       <c r="C37" t="inlineStr">
         <is>
-          <t xml:space="preserve">  5.00 [5.00, 6.00]</t>
+          <t>140.00 [122.50, 158.00]</t>
         </is>
       </c>
       <c r="D37" t="inlineStr">
         <is>
-          <t xml:space="preserve">  5.00 [5.00, 6.00]</t>
+          <t>142.00 [130.00, 160.00]</t>
         </is>
       </c>
       <c r="E37" t="inlineStr">
         <is>
-          <t xml:space="preserve">  5.00 [5.00, 6.00]</t>
+          <t>130.00 [120.00, 150.00]</t>
         </is>
       </c>
       <c r="F37" t="inlineStr">
         <is>
-          <t xml:space="preserve"> 0.602</t>
+          <t>&lt;0.001</t>
         </is>
       </c>
       <c r="G37" t="inlineStr">
@@ -1457,14 +1457,14 @@
       </c>
       <c r="H37" t="inlineStr">
         <is>
-          <t xml:space="preserve"> 0.107</t>
+          <t xml:space="preserve"> 0.242</t>
         </is>
       </c>
     </row>
     <row r="38">
       <c r="A38" t="inlineStr">
         <is>
-          <t>Pughpunts_basal (missing values)</t>
+          <t>MidaMelsa_mm (missing values)</t>
         </is>
       </c>
       <c r="C38" t="inlineStr">
@@ -1486,27 +1486,27 @@
     <row r="39">
       <c r="A39" t="inlineStr">
         <is>
-          <t>Urea_mgdL_preIQ (median [IQR])</t>
+          <t>Pughpunts_basal (median [IQR])</t>
         </is>
       </c>
       <c r="C39" t="inlineStr">
         <is>
-          <t xml:space="preserve">  9.00 [5.00, 37.00]</t>
+          <t xml:space="preserve">  5.00 [5.00, 6.00]</t>
         </is>
       </c>
       <c r="D39" t="inlineStr">
         <is>
-          <t xml:space="preserve">  5.00 [4.00, 6.40]</t>
+          <t xml:space="preserve">  5.00 [5.00, 6.00]</t>
         </is>
       </c>
       <c r="E39" t="inlineStr">
         <is>
-          <t xml:space="preserve"> 37.00 [27.00, 47.00]</t>
+          <t xml:space="preserve">  5.00 [5.00, 6.00]</t>
         </is>
       </c>
       <c r="F39" t="inlineStr">
         <is>
-          <t>&lt;0.001</t>
+          <t xml:space="preserve"> 0.573</t>
         </is>
       </c>
       <c r="G39" t="inlineStr">
@@ -1516,14 +1516,14 @@
       </c>
       <c r="H39" t="inlineStr">
         <is>
-          <t xml:space="preserve"> 2.249</t>
+          <t xml:space="preserve"> 0.119</t>
         </is>
       </c>
     </row>
     <row r="40">
       <c r="A40" t="inlineStr">
         <is>
-          <t>Urea_mgdL_preIQ (missing values)</t>
+          <t>Pughpunts_basal (missing values)</t>
         </is>
       </c>
       <c r="C40" t="inlineStr">
@@ -1545,22 +1545,22 @@
     <row r="41">
       <c r="A41" t="inlineStr">
         <is>
-          <t>plaquetes_preIQ (median [IQR])</t>
+          <t>Urea_mgdL_preIQ (median [IQR])</t>
         </is>
       </c>
       <c r="C41" t="inlineStr">
         <is>
-          <t>107.00 [80.00, 155.00]</t>
+          <t xml:space="preserve">  9.00 [5.00, 37.00]</t>
         </is>
       </c>
       <c r="D41" t="inlineStr">
         <is>
-          <t xml:space="preserve"> 95.00 [70.25, 123.00]</t>
+          <t xml:space="preserve">  5.00 [4.00, 6.40]</t>
         </is>
       </c>
       <c r="E41" t="inlineStr">
         <is>
-          <t>134.00 [100.00, 180.00]</t>
+          <t xml:space="preserve"> 37.00 [27.00, 47.00]</t>
         </is>
       </c>
       <c r="F41" t="inlineStr">
@@ -1575,14 +1575,14 @@
       </c>
       <c r="H41" t="inlineStr">
         <is>
-          <t xml:space="preserve"> 0.749</t>
+          <t xml:space="preserve"> 2.236</t>
         </is>
       </c>
     </row>
     <row r="42">
       <c r="A42" t="inlineStr">
         <is>
-          <t>plaquetes_preIQ (missing values)</t>
+          <t>Urea_mgdL_preIQ (missing values)</t>
         </is>
       </c>
       <c r="C42" t="inlineStr">
@@ -1604,265 +1604,265 @@
     <row r="43">
       <c r="A43" t="inlineStr">
         <is>
-          <t>BBprevis (%)</t>
-        </is>
-      </c>
-      <c r="B43" t="inlineStr">
-        <is>
-          <t>carvedilol</t>
+          <t>hvpg (median [IQR])</t>
         </is>
       </c>
       <c r="C43" t="inlineStr">
         <is>
-          <t xml:space="preserve">    13 ( 3.5) </t>
+          <t xml:space="preserve"> 16.50 [13.00, 20.00]</t>
         </is>
       </c>
       <c r="D43" t="inlineStr">
         <is>
-          <t xml:space="preserve">     1 (  0.5) </t>
+          <t xml:space="preserve"> 17.00 [14.00, 20.50]</t>
         </is>
       </c>
       <c r="E43" t="inlineStr">
         <is>
-          <t xml:space="preserve">    12 ( 6.8) </t>
+          <t xml:space="preserve"> 15.50 [11.00, 19.00]</t>
+        </is>
+      </c>
+      <c r="F43" t="inlineStr">
+        <is>
+          <t>&lt;0.001</t>
+        </is>
+      </c>
+      <c r="G43" t="inlineStr">
+        <is>
+          <t>nonnorm</t>
+        </is>
+      </c>
+      <c r="H43" t="inlineStr">
+        <is>
+          <t xml:space="preserve"> 0.516</t>
         </is>
       </c>
     </row>
     <row r="44">
-      <c r="B44" t="inlineStr">
-        <is>
-          <t>no BB</t>
+      <c r="A44" t="inlineStr">
+        <is>
+          <t>hvpg (missing values)</t>
         </is>
       </c>
       <c r="C44" t="inlineStr">
         <is>
-          <t xml:space="preserve">   341 (91.9) </t>
+          <t>0</t>
         </is>
       </c>
       <c r="D44" t="inlineStr">
         <is>
-          <t xml:space="preserve">   191 ( 98.5) </t>
+          <t>0</t>
         </is>
       </c>
       <c r="E44" t="inlineStr">
         <is>
-          <t xml:space="preserve">   150 (84.7) </t>
-        </is>
-      </c>
-      <c r="F44" t="inlineStr">
+          <t>0</t>
+        </is>
+      </c>
+    </row>
+    <row r="45">
+      <c r="A45" t="inlineStr">
+        <is>
+          <t>plaquetes_preIQ (median [IQR])</t>
+        </is>
+      </c>
+      <c r="C45" t="inlineStr">
+        <is>
+          <t>107.00 [80.00, 155.00]</t>
+        </is>
+      </c>
+      <c r="D45" t="inlineStr">
+        <is>
+          <t xml:space="preserve"> 95.00 [70.25, 123.00]</t>
+        </is>
+      </c>
+      <c r="E45" t="inlineStr">
+        <is>
+          <t>134.00 [100.00, 180.00]</t>
+        </is>
+      </c>
+      <c r="F45" t="inlineStr">
         <is>
           <t>&lt;0.001</t>
         </is>
       </c>
-      <c r="H44" t="inlineStr">
-        <is>
-          <t xml:space="preserve"> 0.511</t>
-        </is>
-      </c>
-    </row>
-    <row r="45">
-      <c r="B45" t="inlineStr">
-        <is>
-          <t>propranolol-nadolol</t>
-        </is>
-      </c>
-      <c r="C45" t="inlineStr">
-        <is>
-          <t xml:space="preserve">    17 ( 4.6) </t>
-        </is>
-      </c>
-      <c r="D45" t="inlineStr">
-        <is>
-          <t xml:space="preserve">     2 (  1.0) </t>
-        </is>
-      </c>
-      <c r="E45" t="inlineStr">
-        <is>
-          <t xml:space="preserve">    15 ( 8.5) </t>
+      <c r="G45" t="inlineStr">
+        <is>
+          <t>nonnorm</t>
+        </is>
+      </c>
+      <c r="H45" t="inlineStr">
+        <is>
+          <t xml:space="preserve"> 0.713</t>
         </is>
       </c>
     </row>
     <row r="46">
       <c r="A46" t="inlineStr">
         <is>
-          <t>DIabetes (%)</t>
-        </is>
-      </c>
-      <c r="B46" t="inlineStr">
-        <is>
-          <t>insulina</t>
+          <t>plaquetes_preIQ (missing values)</t>
         </is>
       </c>
       <c r="C46" t="inlineStr">
         <is>
-          <t xml:space="preserve">   127 (34.2) </t>
+          <t>0</t>
         </is>
       </c>
       <c r="D46" t="inlineStr">
         <is>
-          <t xml:space="preserve">    68 ( 35.1) </t>
+          <t>0</t>
         </is>
       </c>
       <c r="E46" t="inlineStr">
         <is>
-          <t xml:space="preserve">    59 (33.3) </t>
+          <t>0</t>
         </is>
       </c>
     </row>
     <row r="47">
+      <c r="A47" t="inlineStr">
+        <is>
+          <t>BBprevis (%)</t>
+        </is>
+      </c>
       <c r="B47" t="inlineStr">
         <is>
-          <t>no</t>
+          <t>carvedilol</t>
         </is>
       </c>
       <c r="C47" t="inlineStr">
         <is>
-          <t xml:space="preserve">   244 (65.8) </t>
+          <t xml:space="preserve">    14 ( 3.8) </t>
         </is>
       </c>
       <c r="D47" t="inlineStr">
         <is>
-          <t xml:space="preserve">   126 ( 64.9) </t>
+          <t xml:space="preserve">     1 (  0.5) </t>
         </is>
       </c>
       <c r="E47" t="inlineStr">
         <is>
-          <t xml:space="preserve">   118 (66.7) </t>
-        </is>
-      </c>
-      <c r="F47" t="inlineStr">
-        <is>
-          <t xml:space="preserve"> 0.811</t>
-        </is>
-      </c>
-      <c r="H47" t="inlineStr">
-        <is>
-          <t xml:space="preserve"> 0.036</t>
+          <t xml:space="preserve">    13 ( 7.3) </t>
         </is>
       </c>
     </row>
     <row r="48">
-      <c r="A48" t="inlineStr">
-        <is>
-          <t>Enol_Actiu (%)</t>
-        </is>
-      </c>
       <c r="B48" t="inlineStr">
         <is>
-          <t>no</t>
+          <t>no BB</t>
         </is>
       </c>
       <c r="C48" t="inlineStr">
         <is>
-          <t xml:space="preserve">   308 (83.0) </t>
+          <t xml:space="preserve">   340 (91.6) </t>
         </is>
       </c>
       <c r="D48" t="inlineStr">
         <is>
-          <t xml:space="preserve">   158 ( 81.4) </t>
+          <t xml:space="preserve">   191 ( 98.5) </t>
         </is>
       </c>
       <c r="E48" t="inlineStr">
         <is>
-          <t xml:space="preserve">   150 (84.7) </t>
+          <t xml:space="preserve">   149 (84.2) </t>
         </is>
       </c>
       <c r="F48" t="inlineStr">
         <is>
-          <t xml:space="preserve"> 0.479</t>
+          <t>&lt;0.001</t>
         </is>
       </c>
       <c r="H48" t="inlineStr">
         <is>
-          <t xml:space="preserve"> 0.088</t>
+          <t xml:space="preserve"> 0.525</t>
         </is>
       </c>
     </row>
     <row r="49">
       <c r="B49" t="inlineStr">
         <is>
-          <t>si</t>
+          <t>propranolol-nadolol</t>
         </is>
       </c>
       <c r="C49" t="inlineStr">
         <is>
-          <t xml:space="preserve">    63 (17.0) </t>
+          <t xml:space="preserve">    17 ( 4.6) </t>
         </is>
       </c>
       <c r="D49" t="inlineStr">
         <is>
-          <t xml:space="preserve">    36 ( 18.6) </t>
+          <t xml:space="preserve">     2 (  1.0) </t>
         </is>
       </c>
       <c r="E49" t="inlineStr">
         <is>
-          <t xml:space="preserve">    27 (15.3) </t>
+          <t xml:space="preserve">    15 ( 8.5) </t>
         </is>
       </c>
     </row>
     <row r="50">
       <c r="A50" t="inlineStr">
         <is>
-          <t>FsC_10 (%)</t>
+          <t>DIabetes (%)</t>
         </is>
       </c>
       <c r="B50" t="inlineStr">
         <is>
-          <t>no</t>
+          <t>insulina</t>
         </is>
       </c>
       <c r="C50" t="inlineStr">
         <is>
-          <t xml:space="preserve">    26 ( 7.0) </t>
+          <t xml:space="preserve">   127 (34.2) </t>
         </is>
       </c>
       <c r="D50" t="inlineStr">
         <is>
-          <t xml:space="preserve">     7 (  3.6) </t>
+          <t xml:space="preserve">    68 ( 35.1) </t>
         </is>
       </c>
       <c r="E50" t="inlineStr">
         <is>
-          <t xml:space="preserve">    19 (10.7) </t>
-        </is>
-      </c>
-      <c r="F50" t="inlineStr">
-        <is>
-          <t xml:space="preserve"> 0.013</t>
-        </is>
-      </c>
-      <c r="H50" t="inlineStr">
-        <is>
-          <t xml:space="preserve"> 0.279</t>
+          <t xml:space="preserve">    59 (33.3) </t>
         </is>
       </c>
     </row>
     <row r="51">
       <c r="B51" t="inlineStr">
         <is>
-          <t>si</t>
+          <t>no</t>
         </is>
       </c>
       <c r="C51" t="inlineStr">
         <is>
-          <t xml:space="preserve">   345 (93.0) </t>
+          <t xml:space="preserve">   244 (65.8) </t>
         </is>
       </c>
       <c r="D51" t="inlineStr">
         <is>
-          <t xml:space="preserve">   187 ( 96.4) </t>
+          <t xml:space="preserve">   126 ( 64.9) </t>
         </is>
       </c>
       <c r="E51" t="inlineStr">
         <is>
-          <t xml:space="preserve">   158 (89.3) </t>
+          <t xml:space="preserve">   118 (66.7) </t>
+        </is>
+      </c>
+      <c r="F51" t="inlineStr">
+        <is>
+          <t xml:space="preserve"> 0.811</t>
+        </is>
+      </c>
+      <c r="H51" t="inlineStr">
+        <is>
+          <t xml:space="preserve"> 0.036</t>
         </is>
       </c>
     </row>
     <row r="52">
       <c r="A52" t="inlineStr">
         <is>
-          <t>FsC_15 (%)</t>
+          <t>Enol_Actiu (%)</t>
         </is>
       </c>
       <c r="B52" t="inlineStr">
@@ -1872,27 +1872,27 @@
       </c>
       <c r="C52" t="inlineStr">
         <is>
-          <t xml:space="preserve">   105 (28.3) </t>
+          <t xml:space="preserve">   308 (83.0) </t>
         </is>
       </c>
       <c r="D52" t="inlineStr">
         <is>
-          <t xml:space="preserve">    42 ( 21.6) </t>
+          <t xml:space="preserve">   158 ( 81.4) </t>
         </is>
       </c>
       <c r="E52" t="inlineStr">
         <is>
-          <t xml:space="preserve">    63 (35.6) </t>
+          <t xml:space="preserve">   150 (84.7) </t>
         </is>
       </c>
       <c r="F52" t="inlineStr">
         <is>
-          <t xml:space="preserve"> 0.004</t>
+          <t xml:space="preserve"> 0.479</t>
         </is>
       </c>
       <c r="H52" t="inlineStr">
         <is>
-          <t xml:space="preserve"> 0.312</t>
+          <t xml:space="preserve"> 0.088</t>
         </is>
       </c>
     </row>
@@ -1904,24 +1904,24 @@
       </c>
       <c r="C53" t="inlineStr">
         <is>
-          <t xml:space="preserve">   266 (71.7) </t>
+          <t xml:space="preserve">    63 (17.0) </t>
         </is>
       </c>
       <c r="D53" t="inlineStr">
         <is>
-          <t xml:space="preserve">   152 ( 78.4) </t>
+          <t xml:space="preserve">    36 ( 18.6) </t>
         </is>
       </c>
       <c r="E53" t="inlineStr">
         <is>
-          <t xml:space="preserve">   114 (64.4) </t>
+          <t xml:space="preserve">    27 (15.3) </t>
         </is>
       </c>
     </row>
     <row r="54">
       <c r="A54" t="inlineStr">
         <is>
-          <t>FsC_25 (%)</t>
+          <t>FsC_10 (%)</t>
         </is>
       </c>
       <c r="B54" t="inlineStr">
@@ -1931,27 +1931,27 @@
       </c>
       <c r="C54" t="inlineStr">
         <is>
-          <t xml:space="preserve">   220 (59.3) </t>
+          <t xml:space="preserve">    35 ( 9.4) </t>
         </is>
       </c>
       <c r="D54" t="inlineStr">
         <is>
-          <t xml:space="preserve">    96 ( 49.5) </t>
+          <t xml:space="preserve">    12 (  6.2) </t>
         </is>
       </c>
       <c r="E54" t="inlineStr">
         <is>
-          <t xml:space="preserve">   124 (70.1) </t>
+          <t xml:space="preserve">    23 (13.0) </t>
         </is>
       </c>
       <c r="F54" t="inlineStr">
         <is>
-          <t>&lt;0.001</t>
+          <t xml:space="preserve"> 0.039</t>
         </is>
       </c>
       <c r="H54" t="inlineStr">
         <is>
-          <t xml:space="preserve"> 0.429</t>
+          <t xml:space="preserve"> 0.233</t>
         </is>
       </c>
     </row>
@@ -1963,24 +1963,24 @@
       </c>
       <c r="C55" t="inlineStr">
         <is>
-          <t xml:space="preserve">   151 (40.7) </t>
+          <t xml:space="preserve">   336 (90.6) </t>
         </is>
       </c>
       <c r="D55" t="inlineStr">
         <is>
-          <t xml:space="preserve">    98 ( 50.5) </t>
+          <t xml:space="preserve">   182 ( 93.8) </t>
         </is>
       </c>
       <c r="E55" t="inlineStr">
         <is>
-          <t xml:space="preserve">    53 (29.9) </t>
+          <t xml:space="preserve">   154 (87.0) </t>
         </is>
       </c>
     </row>
     <row r="56">
       <c r="A56" t="inlineStr">
         <is>
-          <t>HCC_prev (%)</t>
+          <t>FsC_15 (%)</t>
         </is>
       </c>
       <c r="B56" t="inlineStr">
@@ -1990,17 +1990,17 @@
       </c>
       <c r="C56" t="inlineStr">
         <is>
-          <t xml:space="preserve">   329 (88.7) </t>
+          <t xml:space="preserve">   100 (27.0) </t>
         </is>
       </c>
       <c r="D56" t="inlineStr">
         <is>
-          <t xml:space="preserve">   188 ( 96.9) </t>
+          <t xml:space="preserve">    33 ( 17.0) </t>
         </is>
       </c>
       <c r="E56" t="inlineStr">
         <is>
-          <t xml:space="preserve">   141 (79.7) </t>
+          <t xml:space="preserve">    67 (37.9) </t>
         </is>
       </c>
       <c r="F56" t="inlineStr">
@@ -2010,7 +2010,7 @@
       </c>
       <c r="H56" t="inlineStr">
         <is>
-          <t xml:space="preserve"> 0.557</t>
+          <t xml:space="preserve"> 0.480</t>
         </is>
       </c>
     </row>
@@ -2022,83 +2022,83 @@
       </c>
       <c r="C57" t="inlineStr">
         <is>
-          <t xml:space="preserve">    42 (11.3) </t>
+          <t xml:space="preserve">   271 (73.0) </t>
         </is>
       </c>
       <c r="D57" t="inlineStr">
         <is>
-          <t xml:space="preserve">     6 (  3.1) </t>
+          <t xml:space="preserve">   161 ( 83.0) </t>
         </is>
       </c>
       <c r="E57" t="inlineStr">
         <is>
-          <t xml:space="preserve">    36 (20.3) </t>
+          <t xml:space="preserve">   110 (62.1) </t>
         </is>
       </c>
     </row>
     <row r="58">
       <c r="A58" t="inlineStr">
         <is>
-          <t>HTA (%)</t>
+          <t>FsC_25 (%)</t>
         </is>
       </c>
       <c r="B58" t="inlineStr">
         <is>
-          <t>IECA</t>
+          <t>no</t>
         </is>
       </c>
       <c r="C58" t="inlineStr">
         <is>
-          <t xml:space="preserve">   194 (52.3) </t>
+          <t xml:space="preserve">   213 (57.4) </t>
         </is>
       </c>
       <c r="D58" t="inlineStr">
         <is>
-          <t xml:space="preserve">    87 ( 44.8) </t>
+          <t xml:space="preserve">    95 ( 49.0) </t>
         </is>
       </c>
       <c r="E58" t="inlineStr">
         <is>
-          <t xml:space="preserve">   107 (60.5) </t>
+          <t xml:space="preserve">   118 (66.7) </t>
+        </is>
+      </c>
+      <c r="F58" t="inlineStr">
+        <is>
+          <t xml:space="preserve"> 0.001</t>
+        </is>
+      </c>
+      <c r="H58" t="inlineStr">
+        <is>
+          <t xml:space="preserve"> 0.364</t>
         </is>
       </c>
     </row>
     <row r="59">
       <c r="B59" t="inlineStr">
         <is>
-          <t>ninguno</t>
+          <t>si</t>
         </is>
       </c>
       <c r="C59" t="inlineStr">
         <is>
-          <t xml:space="preserve">   177 (47.7) </t>
+          <t xml:space="preserve">   158 (42.6) </t>
         </is>
       </c>
       <c r="D59" t="inlineStr">
         <is>
-          <t xml:space="preserve">   107 ( 55.2) </t>
+          <t xml:space="preserve">    99 ( 51.0) </t>
         </is>
       </c>
       <c r="E59" t="inlineStr">
         <is>
-          <t xml:space="preserve">    70 (39.5) </t>
-        </is>
-      </c>
-      <c r="F59" t="inlineStr">
-        <is>
-          <t xml:space="preserve"> 0.004</t>
-        </is>
-      </c>
-      <c r="H59" t="inlineStr">
-        <is>
-          <t xml:space="preserve"> 0.316</t>
+          <t xml:space="preserve">    59 (33.3) </t>
         </is>
       </c>
     </row>
     <row r="60">
       <c r="A60" t="inlineStr">
         <is>
-          <t>HVPG_10 (%)</t>
+          <t>HCC_prev (%)</t>
         </is>
       </c>
       <c r="B60" t="inlineStr">
@@ -2108,17 +2108,17 @@
       </c>
       <c r="C60" t="inlineStr">
         <is>
-          <t xml:space="preserve">    43 (11.6) </t>
+          <t xml:space="preserve">   329 (88.7) </t>
         </is>
       </c>
       <c r="D60" t="inlineStr">
         <is>
-          <t xml:space="preserve">     0 (  0.0) </t>
+          <t xml:space="preserve">   188 ( 96.9) </t>
         </is>
       </c>
       <c r="E60" t="inlineStr">
         <is>
-          <t xml:space="preserve">    43 (24.3) </t>
+          <t xml:space="preserve">   141 (79.7) </t>
         </is>
       </c>
       <c r="F60" t="inlineStr">
@@ -2128,7 +2128,7 @@
       </c>
       <c r="H60" t="inlineStr">
         <is>
-          <t xml:space="preserve"> 0.801</t>
+          <t xml:space="preserve"> 0.557</t>
         </is>
       </c>
     </row>
@@ -2140,83 +2140,83 @@
       </c>
       <c r="C61" t="inlineStr">
         <is>
-          <t xml:space="preserve">   328 (88.4) </t>
+          <t xml:space="preserve">    42 (11.3) </t>
         </is>
       </c>
       <c r="D61" t="inlineStr">
         <is>
-          <t xml:space="preserve">   194 (100.0) </t>
+          <t xml:space="preserve">     6 (  3.1) </t>
         </is>
       </c>
       <c r="E61" t="inlineStr">
         <is>
-          <t xml:space="preserve">   134 (75.7) </t>
+          <t xml:space="preserve">    36 (20.3) </t>
         </is>
       </c>
     </row>
     <row r="62">
       <c r="A62" t="inlineStr">
         <is>
-          <t>HVPG_16 (%)</t>
+          <t>HTA (%)</t>
         </is>
       </c>
       <c r="B62" t="inlineStr">
         <is>
-          <t>no</t>
+          <t>IECA</t>
         </is>
       </c>
       <c r="C62" t="inlineStr">
         <is>
-          <t xml:space="preserve">   169 (45.6) </t>
+          <t xml:space="preserve">   196 (52.8) </t>
         </is>
       </c>
       <c r="D62" t="inlineStr">
         <is>
-          <t xml:space="preserve">    70 ( 36.1) </t>
+          <t xml:space="preserve">    89 ( 45.9) </t>
         </is>
       </c>
       <c r="E62" t="inlineStr">
         <is>
-          <t xml:space="preserve">    99 (55.9) </t>
-        </is>
-      </c>
-      <c r="F62" t="inlineStr">
-        <is>
-          <t>&lt;0.001</t>
-        </is>
-      </c>
-      <c r="H62" t="inlineStr">
-        <is>
-          <t xml:space="preserve"> 0.406</t>
+          <t xml:space="preserve">   107 (60.5) </t>
         </is>
       </c>
     </row>
     <row r="63">
       <c r="B63" t="inlineStr">
         <is>
-          <t>si</t>
+          <t>ninguno</t>
         </is>
       </c>
       <c r="C63" t="inlineStr">
         <is>
-          <t xml:space="preserve">   202 (54.4) </t>
+          <t xml:space="preserve">   175 (47.2) </t>
         </is>
       </c>
       <c r="D63" t="inlineStr">
         <is>
-          <t xml:space="preserve">   124 ( 63.9) </t>
+          <t xml:space="preserve">   105 ( 54.1) </t>
         </is>
       </c>
       <c r="E63" t="inlineStr">
         <is>
-          <t xml:space="preserve">    78 (44.1) </t>
+          <t xml:space="preserve">    70 (39.5) </t>
+        </is>
+      </c>
+      <c r="F63" t="inlineStr">
+        <is>
+          <t xml:space="preserve"> 0.007</t>
+        </is>
+      </c>
+      <c r="H63" t="inlineStr">
+        <is>
+          <t xml:space="preserve"> 0.295</t>
         </is>
       </c>
     </row>
     <row r="64">
       <c r="A64" t="inlineStr">
         <is>
-          <t>HVPG_20 (%)</t>
+          <t>HVPG_10 (%)</t>
         </is>
       </c>
       <c r="B64" t="inlineStr">
@@ -2226,27 +2226,27 @@
       </c>
       <c r="C64" t="inlineStr">
         <is>
-          <t xml:space="preserve">   280 (75.5) </t>
+          <t xml:space="preserve">    52 (14.0) </t>
         </is>
       </c>
       <c r="D64" t="inlineStr">
         <is>
-          <t xml:space="preserve">   136 ( 70.1) </t>
+          <t xml:space="preserve">     0 (  0.0) </t>
         </is>
       </c>
       <c r="E64" t="inlineStr">
         <is>
-          <t xml:space="preserve">   144 (81.4) </t>
+          <t xml:space="preserve">    52 (29.4) </t>
         </is>
       </c>
       <c r="F64" t="inlineStr">
         <is>
-          <t xml:space="preserve"> 0.017</t>
+          <t>&lt;0.001</t>
         </is>
       </c>
       <c r="H64" t="inlineStr">
         <is>
-          <t xml:space="preserve"> 0.265</t>
+          <t xml:space="preserve"> 0.912</t>
         </is>
       </c>
     </row>
@@ -2258,210 +2258,225 @@
       </c>
       <c r="C65" t="inlineStr">
         <is>
-          <t xml:space="preserve">    91 (24.5) </t>
+          <t xml:space="preserve">   319 (86.0) </t>
         </is>
       </c>
       <c r="D65" t="inlineStr">
         <is>
-          <t xml:space="preserve">    58 ( 29.9) </t>
+          <t xml:space="preserve">   194 (100.0) </t>
         </is>
       </c>
       <c r="E65" t="inlineStr">
         <is>
-          <t xml:space="preserve">    33 (18.6) </t>
+          <t xml:space="preserve">   125 (70.6) </t>
         </is>
       </c>
     </row>
     <row r="66">
       <c r="A66" t="inlineStr">
         <is>
-          <t>Pughclasse_basal (%)</t>
+          <t>HVPG_16 (%)</t>
         </is>
       </c>
       <c r="B66" t="inlineStr">
         <is>
-          <t>pugh A</t>
+          <t>no</t>
         </is>
       </c>
       <c r="C66" t="inlineStr">
         <is>
-          <t xml:space="preserve">   320 (86.3) </t>
+          <t xml:space="preserve">   174 (46.9) </t>
         </is>
       </c>
       <c r="D66" t="inlineStr">
         <is>
-          <t xml:space="preserve">   167 ( 86.1) </t>
+          <t xml:space="preserve">    70 ( 36.1) </t>
         </is>
       </c>
       <c r="E66" t="inlineStr">
         <is>
-          <t xml:space="preserve">   153 (86.4) </t>
+          <t xml:space="preserve">   104 (58.8) </t>
         </is>
       </c>
       <c r="F66" t="inlineStr">
         <is>
-          <t xml:space="preserve"> 0.309</t>
+          <t>&lt;0.001</t>
         </is>
       </c>
       <c r="H66" t="inlineStr">
         <is>
-          <t xml:space="preserve"> 0.156</t>
+          <t xml:space="preserve"> 0.466</t>
         </is>
       </c>
     </row>
     <row r="67">
       <c r="B67" t="inlineStr">
         <is>
+          <t>si</t>
+        </is>
+      </c>
+      <c r="C67" t="inlineStr">
+        <is>
+          <t xml:space="preserve">   197 (53.1) </t>
+        </is>
+      </c>
+      <c r="D67" t="inlineStr">
+        <is>
+          <t xml:space="preserve">   124 ( 63.9) </t>
+        </is>
+      </c>
+      <c r="E67" t="inlineStr">
+        <is>
+          <t xml:space="preserve">    73 (41.2) </t>
+        </is>
+      </c>
+    </row>
+    <row r="68">
+      <c r="A68" t="inlineStr">
+        <is>
+          <t>HVPG_20 (%)</t>
+        </is>
+      </c>
+      <c r="B68" t="inlineStr">
+        <is>
+          <t>no</t>
+        </is>
+      </c>
+      <c r="C68" t="inlineStr">
+        <is>
+          <t xml:space="preserve">   280 (75.5) </t>
+        </is>
+      </c>
+      <c r="D68" t="inlineStr">
+        <is>
+          <t xml:space="preserve">   136 ( 70.1) </t>
+        </is>
+      </c>
+      <c r="E68" t="inlineStr">
+        <is>
+          <t xml:space="preserve">   144 (81.4) </t>
+        </is>
+      </c>
+      <c r="F68" t="inlineStr">
+        <is>
+          <t xml:space="preserve"> 0.017</t>
+        </is>
+      </c>
+      <c r="H68" t="inlineStr">
+        <is>
+          <t xml:space="preserve"> 0.265</t>
+        </is>
+      </c>
+    </row>
+    <row r="69">
+      <c r="B69" t="inlineStr">
+        <is>
+          <t>si</t>
+        </is>
+      </c>
+      <c r="C69" t="inlineStr">
+        <is>
+          <t xml:space="preserve">    91 (24.5) </t>
+        </is>
+      </c>
+      <c r="D69" t="inlineStr">
+        <is>
+          <t xml:space="preserve">    58 ( 29.9) </t>
+        </is>
+      </c>
+      <c r="E69" t="inlineStr">
+        <is>
+          <t xml:space="preserve">    33 (18.6) </t>
+        </is>
+      </c>
+    </row>
+    <row r="70">
+      <c r="A70" t="inlineStr">
+        <is>
+          <t>Pughclasse_basal (%)</t>
+        </is>
+      </c>
+      <c r="B70" t="inlineStr">
+        <is>
+          <t>pugh A</t>
+        </is>
+      </c>
+      <c r="C70" t="inlineStr">
+        <is>
+          <t xml:space="preserve">   320 (86.3) </t>
+        </is>
+      </c>
+      <c r="D70" t="inlineStr">
+        <is>
+          <t xml:space="preserve">   167 ( 86.1) </t>
+        </is>
+      </c>
+      <c r="E70" t="inlineStr">
+        <is>
+          <t xml:space="preserve">   153 (86.4) </t>
+        </is>
+      </c>
+      <c r="F70" t="inlineStr">
+        <is>
+          <t xml:space="preserve"> 0.309</t>
+        </is>
+      </c>
+      <c r="H70" t="inlineStr">
+        <is>
+          <t xml:space="preserve"> 0.156</t>
+        </is>
+      </c>
+    </row>
+    <row r="71">
+      <c r="B71" t="inlineStr">
+        <is>
           <t>pugh B</t>
         </is>
       </c>
-      <c r="C67" t="inlineStr">
+      <c r="C71" t="inlineStr">
         <is>
           <t xml:space="preserve">    49 (13.2) </t>
         </is>
       </c>
-      <c r="D67" t="inlineStr">
+      <c r="D71" t="inlineStr">
         <is>
           <t xml:space="preserve">    27 ( 13.9) </t>
         </is>
       </c>
-      <c r="E67" t="inlineStr">
+      <c r="E71" t="inlineStr">
         <is>
           <t xml:space="preserve">    22 (12.4) </t>
-        </is>
-      </c>
-    </row>
-    <row r="68">
-      <c r="B68" t="inlineStr">
-        <is>
-          <t>pugh C</t>
-        </is>
-      </c>
-      <c r="C68" t="inlineStr">
-        <is>
-          <t xml:space="preserve">     2 ( 0.5) </t>
-        </is>
-      </c>
-      <c r="D68" t="inlineStr">
-        <is>
-          <t xml:space="preserve">     0 (  0.0) </t>
-        </is>
-      </c>
-      <c r="E68" t="inlineStr">
-        <is>
-          <t xml:space="preserve">     2 ( 1.1) </t>
-        </is>
-      </c>
-    </row>
-    <row r="69">
-      <c r="A69" t="inlineStr">
-        <is>
-          <t>SignesIndirectes_HTP (%)</t>
-        </is>
-      </c>
-      <c r="B69" t="inlineStr">
-        <is>
-          <t>no</t>
-        </is>
-      </c>
-      <c r="C69" t="inlineStr">
-        <is>
-          <t xml:space="preserve">    64 (17.3) </t>
-        </is>
-      </c>
-      <c r="D69" t="inlineStr">
-        <is>
-          <t xml:space="preserve">     3 (  1.5) </t>
-        </is>
-      </c>
-      <c r="E69" t="inlineStr">
-        <is>
-          <t xml:space="preserve">    61 (34.5) </t>
-        </is>
-      </c>
-      <c r="F69" t="inlineStr">
-        <is>
-          <t>&lt;0.001</t>
-        </is>
-      </c>
-      <c r="H69" t="inlineStr">
-        <is>
-          <t xml:space="preserve"> 0.948</t>
-        </is>
-      </c>
-    </row>
-    <row r="70">
-      <c r="B70" t="inlineStr">
-        <is>
-          <t>si</t>
-        </is>
-      </c>
-      <c r="C70" t="inlineStr">
-        <is>
-          <t xml:space="preserve">   307 (82.7) </t>
-        </is>
-      </c>
-      <c r="D70" t="inlineStr">
-        <is>
-          <t xml:space="preserve">   191 ( 98.5) </t>
-        </is>
-      </c>
-      <c r="E70" t="inlineStr">
-        <is>
-          <t xml:space="preserve">   116 (65.5) </t>
-        </is>
-      </c>
-    </row>
-    <row r="71">
-      <c r="A71" t="inlineStr">
-        <is>
-          <t>TTO_Estatinas (%)</t>
-        </is>
-      </c>
-      <c r="B71" t="inlineStr">
-        <is>
-          <t>altres</t>
-        </is>
-      </c>
-      <c r="C71" t="inlineStr">
-        <is>
-          <t xml:space="preserve">     2 ( 0.5) </t>
-        </is>
-      </c>
-      <c r="D71" t="inlineStr">
-        <is>
-          <t xml:space="preserve">     0 (  0.0) </t>
-        </is>
-      </c>
-      <c r="E71" t="inlineStr">
-        <is>
-          <t xml:space="preserve">     2 ( 1.1) </t>
         </is>
       </c>
     </row>
     <row r="72">
       <c r="B72" t="inlineStr">
         <is>
-          <t>atorvastatina</t>
+          <t>pugh C</t>
         </is>
       </c>
       <c r="C72" t="inlineStr">
         <is>
-          <t xml:space="preserve">    28 ( 7.5) </t>
+          <t xml:space="preserve">     2 ( 0.5) </t>
         </is>
       </c>
       <c r="D72" t="inlineStr">
         <is>
-          <t xml:space="preserve">     8 (  4.1) </t>
+          <t xml:space="preserve">     0 (  0.0) </t>
         </is>
       </c>
       <c r="E72" t="inlineStr">
         <is>
-          <t xml:space="preserve">    20 (11.3) </t>
+          <t xml:space="preserve">     2 ( 1.1) </t>
         </is>
       </c>
     </row>
     <row r="73">
+      <c r="A73" t="inlineStr">
+        <is>
+          <t>SignesIndirectes_HTP (%)</t>
+        </is>
+      </c>
       <c r="B73" t="inlineStr">
         <is>
           <t>no</t>
@@ -2469,17 +2484,17 @@
       </c>
       <c r="C73" t="inlineStr">
         <is>
-          <t xml:space="preserve">   318 (85.7) </t>
+          <t xml:space="preserve">    64 (17.3) </t>
         </is>
       </c>
       <c r="D73" t="inlineStr">
         <is>
-          <t xml:space="preserve">   180 ( 92.8) </t>
+          <t xml:space="preserve">     3 (  1.5) </t>
         </is>
       </c>
       <c r="E73" t="inlineStr">
         <is>
-          <t xml:space="preserve">   138 (78.0) </t>
+          <t xml:space="preserve">    61 (34.5) </t>
         </is>
       </c>
       <c r="F73" t="inlineStr">
@@ -2489,176 +2504,161 @@
       </c>
       <c r="H73" t="inlineStr">
         <is>
-          <t xml:space="preserve"> 0.498</t>
+          <t xml:space="preserve"> 0.948</t>
         </is>
       </c>
     </row>
     <row r="74">
       <c r="B74" t="inlineStr">
         <is>
-          <t>rosuvastatina</t>
+          <t>si</t>
         </is>
       </c>
       <c r="C74" t="inlineStr">
         <is>
+          <t xml:space="preserve">   307 (82.7) </t>
+        </is>
+      </c>
+      <c r="D74" t="inlineStr">
+        <is>
+          <t xml:space="preserve">   191 ( 98.5) </t>
+        </is>
+      </c>
+      <c r="E74" t="inlineStr">
+        <is>
+          <t xml:space="preserve">   116 (65.5) </t>
+        </is>
+      </c>
+    </row>
+    <row r="75">
+      <c r="A75" t="inlineStr">
+        <is>
+          <t>TTO_Estatinas (%)</t>
+        </is>
+      </c>
+      <c r="B75" t="inlineStr">
+        <is>
+          <t>altres</t>
+        </is>
+      </c>
+      <c r="C75" t="inlineStr">
+        <is>
           <t xml:space="preserve">     2 ( 0.5) </t>
         </is>
       </c>
-      <c r="D74" t="inlineStr">
-        <is>
-          <t xml:space="preserve">     2 (  1.0) </t>
-        </is>
-      </c>
-      <c r="E74" t="inlineStr">
-        <is>
-          <t xml:space="preserve">     0 ( 0.0) </t>
-        </is>
-      </c>
-    </row>
-    <row r="75">
-      <c r="B75" t="inlineStr">
-        <is>
-          <t>simvastatina</t>
-        </is>
-      </c>
-      <c r="C75" t="inlineStr">
-        <is>
-          <t xml:space="preserve">    21 ( 5.7) </t>
-        </is>
-      </c>
       <c r="D75" t="inlineStr">
         <is>
-          <t xml:space="preserve">     4 (  2.1) </t>
+          <t xml:space="preserve">     0 (  0.0) </t>
         </is>
       </c>
       <c r="E75" t="inlineStr">
         <is>
-          <t xml:space="preserve">    17 ( 9.6) </t>
+          <t xml:space="preserve">     2 ( 1.1) </t>
         </is>
       </c>
     </row>
     <row r="76">
-      <c r="A76" t="inlineStr">
-        <is>
-          <t>VE_basal (%)</t>
-        </is>
-      </c>
       <c r="B76" t="inlineStr">
         <is>
-          <t>no</t>
+          <t>atorvastatina</t>
         </is>
       </c>
       <c r="C76" t="inlineStr">
         <is>
-          <t xml:space="preserve">   124 (33.4) </t>
+          <t xml:space="preserve">    27 ( 7.3) </t>
         </is>
       </c>
       <c r="D76" t="inlineStr">
         <is>
-          <t xml:space="preserve">     3 (  1.5) </t>
+          <t xml:space="preserve">     7 (  3.6) </t>
         </is>
       </c>
       <c r="E76" t="inlineStr">
         <is>
-          <t xml:space="preserve">   121 (68.4) </t>
-        </is>
-      </c>
-      <c r="F76" t="inlineStr">
-        <is>
-          <t>&lt;0.001</t>
-        </is>
-      </c>
-      <c r="H76" t="inlineStr">
-        <is>
-          <t xml:space="preserve"> 1.964</t>
+          <t xml:space="preserve">    20 (11.3) </t>
         </is>
       </c>
     </row>
     <row r="77">
       <c r="B77" t="inlineStr">
         <is>
-          <t>si</t>
+          <t>no</t>
         </is>
       </c>
       <c r="C77" t="inlineStr">
         <is>
-          <t xml:space="preserve">   247 (66.6) </t>
+          <t xml:space="preserve">   315 (84.9) </t>
         </is>
       </c>
       <c r="D77" t="inlineStr">
         <is>
-          <t xml:space="preserve">   191 ( 98.5) </t>
+          <t xml:space="preserve">   177 ( 91.2) </t>
         </is>
       </c>
       <c r="E77" t="inlineStr">
         <is>
-          <t xml:space="preserve">    56 (31.6) </t>
+          <t xml:space="preserve">   138 (78.0) </t>
+        </is>
+      </c>
+      <c r="F77" t="inlineStr">
+        <is>
+          <t xml:space="preserve"> 0.003</t>
+        </is>
+      </c>
+      <c r="H77" t="inlineStr">
+        <is>
+          <t xml:space="preserve"> 0.418</t>
         </is>
       </c>
     </row>
     <row r="78">
-      <c r="A78" t="inlineStr">
-        <is>
-          <t>VG_fúndiques (%)</t>
-        </is>
-      </c>
       <c r="B78" t="inlineStr">
         <is>
-          <t>no</t>
+          <t>rosuvastatina</t>
         </is>
       </c>
       <c r="C78" t="inlineStr">
         <is>
-          <t xml:space="preserve">   342 (92.2) </t>
+          <t xml:space="preserve">     1 ( 0.3) </t>
         </is>
       </c>
       <c r="D78" t="inlineStr">
         <is>
-          <t xml:space="preserve">   173 ( 89.2) </t>
+          <t xml:space="preserve">     1 (  0.5) </t>
         </is>
       </c>
       <c r="E78" t="inlineStr">
         <is>
-          <t xml:space="preserve">   169 (95.5) </t>
-        </is>
-      </c>
-      <c r="F78" t="inlineStr">
-        <is>
-          <t xml:space="preserve"> 0.039</t>
-        </is>
-      </c>
-      <c r="H78" t="inlineStr">
-        <is>
-          <t xml:space="preserve"> 0.239</t>
+          <t xml:space="preserve">     0 ( 0.0) </t>
         </is>
       </c>
     </row>
     <row r="79">
       <c r="B79" t="inlineStr">
         <is>
-          <t>si</t>
+          <t>simvastatina</t>
         </is>
       </c>
       <c r="C79" t="inlineStr">
         <is>
-          <t xml:space="preserve">    29 ( 7.8) </t>
+          <t xml:space="preserve">    26 ( 7.0) </t>
         </is>
       </c>
       <c r="D79" t="inlineStr">
         <is>
-          <t xml:space="preserve">    21 ( 10.8) </t>
+          <t xml:space="preserve">     9 (  4.6) </t>
         </is>
       </c>
       <c r="E79" t="inlineStr">
         <is>
-          <t xml:space="preserve">     8 ( 4.5) </t>
+          <t xml:space="preserve">    17 ( 9.6) </t>
         </is>
       </c>
     </row>
     <row r="80">
       <c r="A80" t="inlineStr">
         <is>
-          <t>colaterals_shunts (%)</t>
+          <t>VE_basal (%)</t>
         </is>
       </c>
       <c r="B80" t="inlineStr">
@@ -2668,27 +2668,27 @@
       </c>
       <c r="C80" t="inlineStr">
         <is>
-          <t xml:space="preserve">   213 (57.4) </t>
+          <t xml:space="preserve">   125 (33.7) </t>
         </is>
       </c>
       <c r="D80" t="inlineStr">
         <is>
-          <t xml:space="preserve">   103 ( 53.1) </t>
+          <t xml:space="preserve">     3 (  1.5) </t>
         </is>
       </c>
       <c r="E80" t="inlineStr">
         <is>
-          <t xml:space="preserve">   110 (62.1) </t>
+          <t xml:space="preserve">   122 (68.9) </t>
         </is>
       </c>
       <c r="F80" t="inlineStr">
         <is>
-          <t xml:space="preserve"> 0.098</t>
+          <t>&lt;0.001</t>
         </is>
       </c>
       <c r="H80" t="inlineStr">
         <is>
-          <t xml:space="preserve"> 0.184</t>
+          <t xml:space="preserve"> 1.990</t>
         </is>
       </c>
     </row>
@@ -2700,83 +2700,83 @@
       </c>
       <c r="C81" t="inlineStr">
         <is>
-          <t xml:space="preserve">   158 (42.6) </t>
+          <t xml:space="preserve">   246 (66.3) </t>
         </is>
       </c>
       <c r="D81" t="inlineStr">
         <is>
-          <t xml:space="preserve">    91 ( 46.9) </t>
+          <t xml:space="preserve">   191 ( 98.5) </t>
         </is>
       </c>
       <c r="E81" t="inlineStr">
         <is>
-          <t xml:space="preserve">    67 (37.9) </t>
+          <t xml:space="preserve">    55 (31.1) </t>
         </is>
       </c>
     </row>
     <row r="82">
       <c r="A82" t="inlineStr">
         <is>
-          <t>dislipemias (%)</t>
+          <t>VG_fúndiques (%)</t>
         </is>
       </c>
       <c r="B82" t="inlineStr">
         <is>
-          <t>No</t>
+          <t>no</t>
         </is>
       </c>
       <c r="C82" t="inlineStr">
         <is>
-          <t xml:space="preserve">   328 (88.4) </t>
+          <t xml:space="preserve">   343 (92.5) </t>
         </is>
       </c>
       <c r="D82" t="inlineStr">
         <is>
-          <t xml:space="preserve">   167 ( 86.1) </t>
+          <t xml:space="preserve">   173 ( 89.2) </t>
         </is>
       </c>
       <c r="E82" t="inlineStr">
         <is>
-          <t xml:space="preserve">   161 (91.0) </t>
+          <t xml:space="preserve">   170 (96.0) </t>
         </is>
       </c>
       <c r="F82" t="inlineStr">
         <is>
-          <t xml:space="preserve"> 0.192</t>
+          <t xml:space="preserve"> 0.021</t>
         </is>
       </c>
       <c r="H82" t="inlineStr">
         <is>
-          <t xml:space="preserve"> 0.153</t>
+          <t xml:space="preserve"> 0.265</t>
         </is>
       </c>
     </row>
     <row r="83">
       <c r="B83" t="inlineStr">
         <is>
-          <t>Si</t>
+          <t>si</t>
         </is>
       </c>
       <c r="C83" t="inlineStr">
         <is>
-          <t xml:space="preserve">    43 (11.6) </t>
+          <t xml:space="preserve">    28 ( 7.5) </t>
         </is>
       </c>
       <c r="D83" t="inlineStr">
         <is>
-          <t xml:space="preserve">    27 ( 13.9) </t>
+          <t xml:space="preserve">    21 ( 10.8) </t>
         </is>
       </c>
       <c r="E83" t="inlineStr">
         <is>
-          <t xml:space="preserve">    16 ( 9.0) </t>
+          <t xml:space="preserve">     7 ( 4.0) </t>
         </is>
       </c>
     </row>
     <row r="84">
       <c r="A84" t="inlineStr">
         <is>
-          <t>etiol_OH (%)</t>
+          <t>colaterals_shunts (%)</t>
         </is>
       </c>
       <c r="B84" t="inlineStr">
@@ -2786,27 +2786,27 @@
       </c>
       <c r="C84" t="inlineStr">
         <is>
-          <t xml:space="preserve">   260 (70.1) </t>
+          <t xml:space="preserve">   211 (56.9) </t>
         </is>
       </c>
       <c r="D84" t="inlineStr">
         <is>
-          <t xml:space="preserve">   127 ( 65.5) </t>
+          <t xml:space="preserve">   100 ( 51.5) </t>
         </is>
       </c>
       <c r="E84" t="inlineStr">
         <is>
-          <t xml:space="preserve">   133 (75.1) </t>
+          <t xml:space="preserve">   111 (62.7) </t>
         </is>
       </c>
       <c r="F84" t="inlineStr">
         <is>
-          <t xml:space="preserve"> 0.055</t>
+          <t xml:space="preserve"> 0.039</t>
         </is>
       </c>
       <c r="H84" t="inlineStr">
         <is>
-          <t xml:space="preserve"> 0.213</t>
+          <t xml:space="preserve"> 0.227</t>
         </is>
       </c>
     </row>
@@ -2818,132 +2818,152 @@
       </c>
       <c r="C85" t="inlineStr">
         <is>
-          <t xml:space="preserve">   111 (29.9) </t>
+          <t xml:space="preserve">   160 (43.1) </t>
         </is>
       </c>
       <c r="D85" t="inlineStr">
         <is>
-          <t xml:space="preserve">    67 ( 34.5) </t>
+          <t xml:space="preserve">    94 ( 48.5) </t>
         </is>
       </c>
       <c r="E85" t="inlineStr">
         <is>
-          <t xml:space="preserve">    44 (24.9) </t>
+          <t xml:space="preserve">    66 (37.3) </t>
         </is>
       </c>
     </row>
     <row r="86">
       <c r="A86" t="inlineStr">
         <is>
-          <t>etiologiaCH (%)</t>
+          <t>dislipemias (%)</t>
         </is>
       </c>
       <c r="B86" t="inlineStr">
         <is>
-          <t>Altres</t>
+          <t>No</t>
         </is>
       </c>
       <c r="C86" t="inlineStr">
         <is>
-          <t xml:space="preserve">    17 ( 4.6) </t>
+          <t xml:space="preserve">   328 (88.4) </t>
         </is>
       </c>
       <c r="D86" t="inlineStr">
         <is>
-          <t xml:space="preserve">     0 (  0.0) </t>
+          <t xml:space="preserve">   167 ( 86.1) </t>
         </is>
       </c>
       <c r="E86" t="inlineStr">
         <is>
-          <t xml:space="preserve">    17 ( 9.6) </t>
+          <t xml:space="preserve">   161 (91.0) </t>
+        </is>
+      </c>
+      <c r="F86" t="inlineStr">
+        <is>
+          <t xml:space="preserve"> 0.192</t>
+        </is>
+      </c>
+      <c r="H86" t="inlineStr">
+        <is>
+          <t xml:space="preserve"> 0.153</t>
         </is>
       </c>
     </row>
     <row r="87">
       <c r="B87" t="inlineStr">
         <is>
-          <t>Colestàtica?/Autoimmune</t>
+          <t>Si</t>
         </is>
       </c>
       <c r="C87" t="inlineStr">
         <is>
-          <t xml:space="preserve">    10 ( 2.7) </t>
+          <t xml:space="preserve">    43 (11.6) </t>
         </is>
       </c>
       <c r="D87" t="inlineStr">
         <is>
-          <t xml:space="preserve">     0 (  0.0) </t>
+          <t xml:space="preserve">    27 ( 13.9) </t>
         </is>
       </c>
       <c r="E87" t="inlineStr">
         <is>
-          <t xml:space="preserve">    10 ( 5.6) </t>
+          <t xml:space="preserve">    16 ( 9.0) </t>
         </is>
       </c>
     </row>
     <row r="88">
+      <c r="A88" t="inlineStr">
+        <is>
+          <t>etiol_OH (%)</t>
+        </is>
+      </c>
       <c r="B88" t="inlineStr">
         <is>
-          <t>MAFLD</t>
+          <t>no</t>
         </is>
       </c>
       <c r="C88" t="inlineStr">
         <is>
-          <t xml:space="preserve">    39 (10.5) </t>
+          <t xml:space="preserve">   260 (70.1) </t>
         </is>
       </c>
       <c r="D88" t="inlineStr">
         <is>
-          <t xml:space="preserve">    18 (  9.3) </t>
+          <t xml:space="preserve">   127 ( 65.5) </t>
         </is>
       </c>
       <c r="E88" t="inlineStr">
         <is>
-          <t xml:space="preserve">    21 (11.9) </t>
+          <t xml:space="preserve">   133 (75.1) </t>
+        </is>
+      </c>
+      <c r="F88" t="inlineStr">
+        <is>
+          <t xml:space="preserve"> 0.055</t>
+        </is>
+      </c>
+      <c r="H88" t="inlineStr">
+        <is>
+          <t xml:space="preserve"> 0.213</t>
         </is>
       </c>
     </row>
     <row r="89">
       <c r="B89" t="inlineStr">
         <is>
-          <t>OH</t>
+          <t>si</t>
         </is>
       </c>
       <c r="C89" t="inlineStr">
         <is>
-          <t xml:space="preserve">    76 (20.5) </t>
+          <t xml:space="preserve">   111 (29.9) </t>
         </is>
       </c>
       <c r="D89" t="inlineStr">
         <is>
-          <t xml:space="preserve">    47 ( 24.2) </t>
+          <t xml:space="preserve">    67 ( 34.5) </t>
         </is>
       </c>
       <c r="E89" t="inlineStr">
         <is>
-          <t xml:space="preserve">    29 (16.4) </t>
-        </is>
-      </c>
-      <c r="F89" t="inlineStr">
-        <is>
-          <t>&lt;0.001</t>
-        </is>
-      </c>
-      <c r="H89" t="inlineStr">
-        <is>
-          <t xml:space="preserve"> 0.778</t>
+          <t xml:space="preserve">    44 (24.9) </t>
         </is>
       </c>
     </row>
     <row r="90">
+      <c r="A90" t="inlineStr">
+        <is>
+          <t>etiologiaCH (%)</t>
+        </is>
+      </c>
       <c r="B90" t="inlineStr">
         <is>
-          <t>OH+MAFLD</t>
+          <t>Altres</t>
         </is>
       </c>
       <c r="C90" t="inlineStr">
         <is>
-          <t xml:space="preserve">     9 ( 2.4) </t>
+          <t xml:space="preserve">    17 ( 4.6) </t>
         </is>
       </c>
       <c r="D90" t="inlineStr">
@@ -2953,218 +2973,198 @@
       </c>
       <c r="E90" t="inlineStr">
         <is>
-          <t xml:space="preserve">     9 ( 5.1) </t>
+          <t xml:space="preserve">    17 ( 9.6) </t>
         </is>
       </c>
     </row>
     <row r="91">
       <c r="B91" t="inlineStr">
         <is>
-          <t>OH+Virus</t>
+          <t>Colestàtica?/Autoimmune</t>
         </is>
       </c>
       <c r="C91" t="inlineStr">
         <is>
-          <t xml:space="preserve">    26 ( 7.0) </t>
+          <t xml:space="preserve">    10 ( 2.7) </t>
         </is>
       </c>
       <c r="D91" t="inlineStr">
         <is>
-          <t xml:space="preserve">    20 ( 10.3) </t>
+          <t xml:space="preserve">     0 (  0.0) </t>
         </is>
       </c>
       <c r="E91" t="inlineStr">
         <is>
-          <t xml:space="preserve">     6 ( 3.4) </t>
+          <t xml:space="preserve">    10 ( 5.6) </t>
         </is>
       </c>
     </row>
     <row r="92">
       <c r="B92" t="inlineStr">
         <is>
-          <t>Virus</t>
+          <t>MAFLD</t>
         </is>
       </c>
       <c r="C92" t="inlineStr">
         <is>
-          <t xml:space="preserve">   194 (52.3) </t>
+          <t xml:space="preserve">    39 (10.5) </t>
         </is>
       </c>
       <c r="D92" t="inlineStr">
         <is>
-          <t xml:space="preserve">   109 ( 56.2) </t>
+          <t xml:space="preserve">    18 (  9.3) </t>
         </is>
       </c>
       <c r="E92" t="inlineStr">
         <is>
-          <t xml:space="preserve">    85 (48.0) </t>
+          <t xml:space="preserve">    21 (11.9) </t>
         </is>
       </c>
     </row>
     <row r="93">
-      <c r="A93" t="inlineStr">
-        <is>
-          <t>respostHDK_aguda (%)</t>
-        </is>
-      </c>
       <c r="B93" t="inlineStr">
         <is>
-          <t>no</t>
+          <t>OH</t>
         </is>
       </c>
       <c r="C93" t="inlineStr">
         <is>
-          <t xml:space="preserve">   123 (33.2) </t>
+          <t xml:space="preserve">    76 (20.5) </t>
         </is>
       </c>
       <c r="D93" t="inlineStr">
         <is>
-          <t xml:space="preserve">    62 ( 32.0) </t>
+          <t xml:space="preserve">    47 ( 24.2) </t>
         </is>
       </c>
       <c r="E93" t="inlineStr">
         <is>
-          <t xml:space="preserve">    61 (34.5) </t>
+          <t xml:space="preserve">    29 (16.4) </t>
         </is>
       </c>
       <c r="F93" t="inlineStr">
         <is>
-          <t xml:space="preserve"> 0.688</t>
+          <t>&lt;0.001</t>
         </is>
       </c>
       <c r="H93" t="inlineStr">
         <is>
-          <t xml:space="preserve"> 0.053</t>
+          <t xml:space="preserve"> 0.778</t>
         </is>
       </c>
     </row>
     <row r="94">
       <c r="B94" t="inlineStr">
         <is>
-          <t>si</t>
+          <t>OH+MAFLD</t>
         </is>
       </c>
       <c r="C94" t="inlineStr">
         <is>
-          <t xml:space="preserve">   248 (66.8) </t>
+          <t xml:space="preserve">     9 ( 2.4) </t>
         </is>
       </c>
       <c r="D94" t="inlineStr">
         <is>
-          <t xml:space="preserve">   132 ( 68.0) </t>
+          <t xml:space="preserve">     0 (  0.0) </t>
         </is>
       </c>
       <c r="E94" t="inlineStr">
         <is>
-          <t xml:space="preserve">   116 (65.5) </t>
+          <t xml:space="preserve">     9 ( 5.1) </t>
         </is>
       </c>
     </row>
     <row r="95">
-      <c r="A95" t="inlineStr">
-        <is>
-          <t>respostHDK_crònica (%)</t>
-        </is>
-      </c>
       <c r="B95" t="inlineStr">
         <is>
-          <t>no</t>
+          <t>OH+Virus</t>
         </is>
       </c>
       <c r="C95" t="inlineStr">
         <is>
-          <t xml:space="preserve">   143 (38.5) </t>
+          <t xml:space="preserve">    26 ( 7.0) </t>
         </is>
       </c>
       <c r="D95" t="inlineStr">
         <is>
-          <t xml:space="preserve">    74 ( 38.1) </t>
+          <t xml:space="preserve">    20 ( 10.3) </t>
         </is>
       </c>
       <c r="E95" t="inlineStr">
         <is>
-          <t xml:space="preserve">    69 (39.0) </t>
-        </is>
-      </c>
-      <c r="F95" t="inlineStr">
-        <is>
-          <t xml:space="preserve"> 0.953</t>
-        </is>
-      </c>
-      <c r="H95" t="inlineStr">
-        <is>
-          <t xml:space="preserve"> 0.017</t>
+          <t xml:space="preserve">     6 ( 3.4) </t>
         </is>
       </c>
     </row>
     <row r="96">
       <c r="B96" t="inlineStr">
         <is>
-          <t>si</t>
+          <t>Virus</t>
         </is>
       </c>
       <c r="C96" t="inlineStr">
         <is>
-          <t xml:space="preserve">   228 (61.5) </t>
+          <t xml:space="preserve">   194 (52.3) </t>
         </is>
       </c>
       <c r="D96" t="inlineStr">
         <is>
-          <t xml:space="preserve">   120 ( 61.9) </t>
+          <t xml:space="preserve">   109 ( 56.2) </t>
         </is>
       </c>
       <c r="E96" t="inlineStr">
         <is>
-          <t xml:space="preserve">   108 (61.0) </t>
+          <t xml:space="preserve">    85 (48.0) </t>
         </is>
       </c>
     </row>
     <row r="97">
       <c r="A97" t="inlineStr">
         <is>
-          <t>ttBBNS_Cronic (%)</t>
+          <t>presenciaCSPH (%)</t>
         </is>
       </c>
       <c r="B97" t="inlineStr">
         <is>
-          <t>carvedilol</t>
+          <t>indeterminat</t>
         </is>
       </c>
       <c r="C97" t="inlineStr">
         <is>
-          <t xml:space="preserve">    77 (20.8) </t>
+          <t xml:space="preserve">    67 (18.1) </t>
         </is>
       </c>
       <c r="D97" t="inlineStr">
         <is>
-          <t xml:space="preserve">    65 ( 33.5) </t>
+          <t xml:space="preserve">     0 (  0.0) </t>
         </is>
       </c>
       <c r="E97" t="inlineStr">
         <is>
-          <t xml:space="preserve">    12 ( 6.8) </t>
+          <t xml:space="preserve">    67 (37.9) </t>
         </is>
       </c>
     </row>
     <row r="98">
       <c r="B98" t="inlineStr">
         <is>
-          <t>no BB</t>
+          <t>no CSPH</t>
         </is>
       </c>
       <c r="C98" t="inlineStr">
         <is>
-          <t xml:space="preserve">   154 (41.5) </t>
+          <t xml:space="preserve">    47 (12.7) </t>
         </is>
       </c>
       <c r="D98" t="inlineStr">
         <is>
-          <t xml:space="preserve">     6 (  3.1) </t>
+          <t xml:space="preserve">     0 (  0.0) </t>
         </is>
       </c>
       <c r="E98" t="inlineStr">
         <is>
-          <t xml:space="preserve">   148 (83.6) </t>
+          <t xml:space="preserve">    47 (26.6) </t>
         </is>
       </c>
       <c r="F98" t="inlineStr">
@@ -3174,29 +3174,228 @@
       </c>
       <c r="H98" t="inlineStr">
         <is>
-          <t xml:space="preserve"> 2.791</t>
+          <t xml:space="preserve"> 1.902</t>
         </is>
       </c>
     </row>
     <row r="99">
       <c r="B99" t="inlineStr">
         <is>
+          <t>si CSPH</t>
+        </is>
+      </c>
+      <c r="C99" t="inlineStr">
+        <is>
+          <t xml:space="preserve">   257 (69.3) </t>
+        </is>
+      </c>
+      <c r="D99" t="inlineStr">
+        <is>
+          <t xml:space="preserve">   194 (100.0) </t>
+        </is>
+      </c>
+      <c r="E99" t="inlineStr">
+        <is>
+          <t xml:space="preserve">    63 (35.6) </t>
+        </is>
+      </c>
+    </row>
+    <row r="100">
+      <c r="A100" t="inlineStr">
+        <is>
+          <t>respostHDK_aguda (%)</t>
+        </is>
+      </c>
+      <c r="B100" t="inlineStr">
+        <is>
+          <t>no</t>
+        </is>
+      </c>
+      <c r="C100" t="inlineStr">
+        <is>
+          <t xml:space="preserve">   132 (35.6) </t>
+        </is>
+      </c>
+      <c r="D100" t="inlineStr">
+        <is>
+          <t xml:space="preserve">    60 ( 30.9) </t>
+        </is>
+      </c>
+      <c r="E100" t="inlineStr">
+        <is>
+          <t xml:space="preserve">    72 (40.7) </t>
+        </is>
+      </c>
+      <c r="F100" t="inlineStr">
+        <is>
+          <t xml:space="preserve"> 0.064</t>
+        </is>
+      </c>
+      <c r="H100" t="inlineStr">
+        <is>
+          <t xml:space="preserve"> 0.204</t>
+        </is>
+      </c>
+    </row>
+    <row r="101">
+      <c r="B101" t="inlineStr">
+        <is>
+          <t>si</t>
+        </is>
+      </c>
+      <c r="C101" t="inlineStr">
+        <is>
+          <t xml:space="preserve">   239 (64.4) </t>
+        </is>
+      </c>
+      <c r="D101" t="inlineStr">
+        <is>
+          <t xml:space="preserve">   134 ( 69.1) </t>
+        </is>
+      </c>
+      <c r="E101" t="inlineStr">
+        <is>
+          <t xml:space="preserve">   105 (59.3) </t>
+        </is>
+      </c>
+    </row>
+    <row r="102">
+      <c r="A102" t="inlineStr">
+        <is>
+          <t>respostHDK_crònica (%)</t>
+        </is>
+      </c>
+      <c r="B102" t="inlineStr">
+        <is>
+          <t>no</t>
+        </is>
+      </c>
+      <c r="C102" t="inlineStr">
+        <is>
+          <t xml:space="preserve">   141 (38.0) </t>
+        </is>
+      </c>
+      <c r="D102" t="inlineStr">
+        <is>
+          <t xml:space="preserve">    73 ( 37.6) </t>
+        </is>
+      </c>
+      <c r="E102" t="inlineStr">
+        <is>
+          <t xml:space="preserve">    68 (38.4) </t>
+        </is>
+      </c>
+      <c r="F102" t="inlineStr">
+        <is>
+          <t xml:space="preserve"> 0.961</t>
+        </is>
+      </c>
+      <c r="H102" t="inlineStr">
+        <is>
+          <t xml:space="preserve"> 0.016</t>
+        </is>
+      </c>
+    </row>
+    <row r="103">
+      <c r="B103" t="inlineStr">
+        <is>
+          <t>si</t>
+        </is>
+      </c>
+      <c r="C103" t="inlineStr">
+        <is>
+          <t xml:space="preserve">   230 (62.0) </t>
+        </is>
+      </c>
+      <c r="D103" t="inlineStr">
+        <is>
+          <t xml:space="preserve">   121 ( 62.4) </t>
+        </is>
+      </c>
+      <c r="E103" t="inlineStr">
+        <is>
+          <t xml:space="preserve">   109 (61.6) </t>
+        </is>
+      </c>
+    </row>
+    <row r="104">
+      <c r="A104" t="inlineStr">
+        <is>
+          <t>ttBBNS_Cronic (%)</t>
+        </is>
+      </c>
+      <c r="B104" t="inlineStr">
+        <is>
+          <t>carvedilol</t>
+        </is>
+      </c>
+      <c r="C104" t="inlineStr">
+        <is>
+          <t xml:space="preserve">    77 (20.8) </t>
+        </is>
+      </c>
+      <c r="D104" t="inlineStr">
+        <is>
+          <t xml:space="preserve">    65 ( 33.5) </t>
+        </is>
+      </c>
+      <c r="E104" t="inlineStr">
+        <is>
+          <t xml:space="preserve">    12 ( 6.8) </t>
+        </is>
+      </c>
+    </row>
+    <row r="105">
+      <c r="B105" t="inlineStr">
+        <is>
+          <t>no BB</t>
+        </is>
+      </c>
+      <c r="C105" t="inlineStr">
+        <is>
+          <t xml:space="preserve">   153 (41.2) </t>
+        </is>
+      </c>
+      <c r="D105" t="inlineStr">
+        <is>
+          <t xml:space="preserve">     6 (  3.1) </t>
+        </is>
+      </c>
+      <c r="E105" t="inlineStr">
+        <is>
+          <t xml:space="preserve">   147 (83.1) </t>
+        </is>
+      </c>
+      <c r="F105" t="inlineStr">
+        <is>
+          <t>&lt;0.001</t>
+        </is>
+      </c>
+      <c r="H105" t="inlineStr">
+        <is>
+          <t xml:space="preserve"> 2.739</t>
+        </is>
+      </c>
+    </row>
+    <row r="106">
+      <c r="B106" t="inlineStr">
+        <is>
           <t>propranolol-nadolol</t>
         </is>
       </c>
-      <c r="C99" t="inlineStr">
-        <is>
-          <t xml:space="preserve">   140 (37.7) </t>
-        </is>
-      </c>
-      <c r="D99" t="inlineStr">
+      <c r="C106" t="inlineStr">
+        <is>
+          <t xml:space="preserve">   141 (38.0) </t>
+        </is>
+      </c>
+      <c r="D106" t="inlineStr">
         <is>
           <t xml:space="preserve">   123 ( 63.4) </t>
         </is>
       </c>
-      <c r="E99" t="inlineStr">
-        <is>
-          <t xml:space="preserve">    17 ( 9.6) </t>
+      <c r="E106" t="inlineStr">
+        <is>
+          <t xml:space="preserve">    18 (10.2) </t>
         </is>
       </c>
     </row>

</xml_diff>